<commit_message>
calapan and latest updates
</commit_message>
<xml_diff>
--- a/Enduse List.xlsx
+++ b/Enduse List.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="261">
   <si>
     <t>ENDUSE LIST</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>69KV Pole No. 3 and 4</t>
+  </si>
+  <si>
+    <t>750kVA Transformer</t>
   </si>
   <si>
     <t>750KVA Transformer Protection Relay</t>
@@ -166,6 +169,9 @@
 </t>
   </si>
   <si>
+    <t>Common Bus Differential Fault &amp; Breaker Failure</t>
+  </si>
+  <si>
     <t>Community</t>
   </si>
   <si>
@@ -175,6 +181,9 @@
     <t>Computer/Electronic device power supply</t>
   </si>
   <si>
+    <t>Conference Room</t>
+  </si>
+  <si>
     <t>Control Air Compressor - Common</t>
   </si>
   <si>
@@ -229,7 +238,7 @@
     <t>Deep Well Riser Pipes Pull-out</t>
   </si>
   <si>
-    <t>DG No. 1&amp;2</t>
+    <t>DG 1 and 2</t>
   </si>
   <si>
     <t>DG Unit 4 Linkage Clamp</t>
@@ -239,7 +248,7 @@
 </t>
   </si>
   <si>
-    <t>DG1(CV Area) Main Engine Parts &amp; Components</t>
+    <t>DG1 (CV Area) Main Engine Parts &amp; Components</t>
   </si>
   <si>
     <t xml:space="preserve">DG2
@@ -300,9 +309,6 @@
     <t>Fabrication of Powerhouse Ventilation Louvers</t>
   </si>
   <si>
-    <t>Fabrication of Unit 4 Starting Valve Relief Valve Blind Plug</t>
-  </si>
-  <si>
     <t>Facilities Improvement</t>
   </si>
   <si>
@@ -364,6 +370,9 @@
   </si>
   <si>
     <t>Generator Unit 2</t>
+  </si>
+  <si>
+    <t>Generator Unit 4</t>
   </si>
   <si>
     <t>Grounding System Lay-out / Installation</t>
@@ -449,9 +458,6 @@
 </t>
   </si>
   <si>
-    <t>lant Common Tools, Special Tools and Equipments</t>
-  </si>
-  <si>
     <t>Lifting Equipment for Transferring of Heavy Parts/Boxes with Parts</t>
   </si>
   <si>
@@ -576,6 +582,9 @@
     <t>Pielstick Jacket Liner</t>
   </si>
   <si>
+    <t>Plant Common Tools, Special Tools and Equipment</t>
+  </si>
+  <si>
     <t>Plant Common Tools, Special Tools, and Equipment</t>
   </si>
   <si>
@@ -684,6 +693,9 @@
     <t>Spare Stator</t>
   </si>
   <si>
+    <t>Spare Stator Rewinding Enclosure</t>
+  </si>
+  <si>
     <t>Staffhouse 1 - Site</t>
   </si>
   <si>
@@ -696,6 +708,9 @@
     <t>Starting Air Compressor - Common</t>
   </si>
   <si>
+    <t>Starting Air Compressor - Pielstick</t>
+  </si>
+  <si>
     <t>Starting Air Compressor No. 1</t>
   </si>
   <si>
@@ -706,9 +721,6 @@
   </si>
   <si>
     <t>Starting Air Compressor No. 4</t>
-  </si>
-  <si>
-    <t>Starting Air Compressor No. 4 &amp; 5</t>
   </si>
   <si>
     <t>Starting Air Compressor No. 5</t>
@@ -752,6 +764,9 @@
     <t>Testing of 750KVA Transformer</t>
   </si>
   <si>
+    <t>Tools, Inventory-Mary Grace Bugna</t>
+  </si>
+  <si>
     <t>Toyota Inova</t>
   </si>
   <si>
@@ -759,6 +774,9 @@
   </si>
   <si>
     <t>Trainees on Oil Spill</t>
+  </si>
+  <si>
+    <t>Turbo Charger Air Intake</t>
   </si>
   <si>
     <t>Turning Gear Motor DG 1-3</t>
@@ -1183,10 +1201,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B255"/>
+  <dimension ref="A1:B261"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B255" sqref="B255"/>
+      <selection activeCell="B261" sqref="B261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2389,7 +2407,7 @@
         <v>148</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2397,7 +2415,7 @@
         <v>149</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -3230,6 +3248,54 @@
       </c>
       <c r="B255" s="2" t="s">
         <v>254</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="A256" s="5">
+        <v>254</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257" s="5">
+        <v>255</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258" s="5">
+        <v>256</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259" s="5">
+        <v>257</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
+      <c r="A260" s="5">
+        <v>258</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
+      <c r="A261" s="5">
+        <v>259</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>